<commit_message>
Updated daily stand-up meeting templet
</commit_message>
<xml_diff>
--- a/Project_Files/Gdp-02-Sprint01/Stand-up Meeting Sec03Team05 Sprint01.xlsx
+++ b/Project_Files/Gdp-02-Sprint01/Stand-up Meeting Sec03Team05 Sprint01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gopin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Gdp-02-Sprint01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8768032-7FCE-43B6-8DA9-FF872B0EAF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E34578-0257-4D13-83F7-A763CDBC05C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="420" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -138,6 +138,24 @@
     <t>1. What did I accomplish?       
 2.What will I do today?
 3.What obstacles are impeding my progress?</t>
+  </si>
+  <si>
+    <t>1) Had Discussion with Team on GDP2 Project works</t>
+  </si>
+  <si>
+    <t>2)  Discussed with team about the work, tasks pending and set milestones for each activity.</t>
+  </si>
+  <si>
+    <t>1)completed discussion with Team and finalized workflow.</t>
+  </si>
+  <si>
+    <t>2) I will fix the code for new table name in backend and write code for the Eventdeleterequest activity.</t>
+  </si>
+  <si>
+    <t>1) I have reviwed backend code for Eventdeleterequest activity</t>
+  </si>
+  <si>
+    <t>2) I will write backend code for Eventdeleterequest activity.</t>
   </si>
 </sst>
 </file>
@@ -730,15 +748,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="6" width="34.5546875" customWidth="1"/>
-    <col min="7" max="26" width="8.88671875" customWidth="1"/>
+    <col min="2" max="6" width="34.54296875" customWidth="1"/>
+    <col min="7" max="26" width="8.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
@@ -1127,9 +1145,15 @@
       <c r="A14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1155,9 +1179,15 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
       <c r="A15" s="9"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1183,10 +1213,14 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
       <c r="A16" s="10"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
-        <v>3</v>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>

</xml_diff>